<commit_message>
Updated Vehicle_Matrix's Tesla section
</commit_message>
<xml_diff>
--- a/doc/Vehicle_Matrix.xlsx
+++ b/doc/Vehicle_Matrix.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD87490B-D4BF-4B0D-AF17-0161D5B0BD4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\PC\Misc\Documents\CIS255_Vehicle\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44CEED0-DA3B-4C53-B750-2C0AAF68D8DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="42">
   <si>
     <t>Make</t>
   </si>
@@ -147,22 +152,13 @@
     <t>Tesla</t>
   </si>
   <si>
-    <t>Cybertruck</t>
-  </si>
-  <si>
     <t>Model S</t>
   </si>
   <si>
     <t>Model 3</t>
   </si>
   <si>
-    <t>Standard</t>
-  </si>
-  <si>
-    <t>Mid Range</t>
-  </si>
-  <si>
-    <t>Performance</t>
+    <t>Model x</t>
   </si>
 </sst>
 </file>
@@ -784,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
@@ -1473,10 +1469,10 @@
         <v>8</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D30" s="21">
-        <v>0</v>
+        <v>2019</v>
       </c>
       <c r="E30" s="21" t="s">
         <v>18</v>
@@ -1485,7 +1481,7 @@
         <v>4</v>
       </c>
       <c r="G30" s="22" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1496,10 +1492,10 @@
         <v>8</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D31" s="21">
-        <v>0</v>
+        <v>2018</v>
       </c>
       <c r="E31" s="21" t="s">
         <v>18</v>
@@ -1508,7 +1504,7 @@
         <v>4</v>
       </c>
       <c r="G31" s="22" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1519,7 +1515,7 @@
         <v>14</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D32" s="21">
         <v>2021</v>
@@ -1542,7 +1538,7 @@
         <v>14</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D33" s="21">
         <v>2021</v>
@@ -1565,13 +1561,13 @@
         <v>20</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D34" s="21">
         <v>2020</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="F34" s="21">
         <v>4</v>
@@ -1588,13 +1584,13 @@
         <v>20</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D35" s="21">
         <v>2020</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="F35" s="21">
         <v>4</v>
@@ -1611,19 +1607,19 @@
         <v>20</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D36" s="24">
         <v>2020</v>
       </c>
-      <c r="E36" s="24" t="s">
-        <v>44</v>
+      <c r="E36" s="21" t="s">
+        <v>18</v>
       </c>
       <c r="F36" s="24">
         <v>4</v>
       </c>
       <c r="G36" s="25" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revised errors in data
</commit_message>
<xml_diff>
--- a/doc/Vehicle_Matrix.xlsx
+++ b/doc/Vehicle_Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\PC\Misc\Documents\CIS255_Vehicle\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44CEED0-DA3B-4C53-B750-2C0AAF68D8DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E76B63-A76B-40E9-9555-21A32DE6D3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -780,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
@@ -1041,7 +1041,7 @@
         <v>10</v>
       </c>
       <c r="F11" s="12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>13</v>
@@ -1202,7 +1202,7 @@
         <v>10</v>
       </c>
       <c r="F18" s="15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G18" s="16" t="s">
         <v>29</v>
@@ -1363,7 +1363,7 @@
         <v>10</v>
       </c>
       <c r="F25" s="18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G25" s="19" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
-Modified and added files needed for Task 1 completion
-Updated Vehicle_Matrix based on student workshop comments and final check

-Updated help files based on visio png and project file addition
</commit_message>
<xml_diff>
--- a/doc/Vehicle_Matrix.xlsx
+++ b/doc/Vehicle_Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\PC\Misc\Documents\CIS255_Vehicle\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDDE44D7-73B8-45C5-9E3E-1877CCD75C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256B3944-1755-4C06-BD82-0045347248B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="55">
   <si>
     <t>Make</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>Model Y</t>
+  </si>
+  <si>
+    <t>Gr86</t>
   </si>
 </sst>
 </file>
@@ -260,7 +263,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -391,39 +394,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -525,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -585,6 +555,96 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -594,94 +654,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1000,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
@@ -1017,55 +996,55 @@
     <col min="16384" max="16384" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="52" t="s">
+      <c r="F1" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="48" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="55">
         <v>2018</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="17">
+      <c r="F2" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="55">
         <v>2</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="54" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1190,7 +1169,7 @@
         <v>2015</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="G7" s="18">
         <v>4</v>
@@ -1242,7 +1221,7 @@
         <v>2019</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G9" s="18">
         <v>2</v>
@@ -1252,54 +1231,54 @@
       </c>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="58">
         <v>2020</v>
       </c>
-      <c r="F10" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="25">
+      <c r="F10" s="57" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="58">
         <v>2</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="57" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="27" t="s">
+      <c r="C11" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="25">
         <v>2018</v>
       </c>
-      <c r="F11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="28">
-        <v>4</v>
-      </c>
-      <c r="H11" s="27" t="s">
+      <c r="F11" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="25">
+        <v>4</v>
+      </c>
+      <c r="H11" s="24" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1363,7 +1342,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>27</v>
@@ -1441,7 +1420,7 @@
         <v>20</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>28</v>
@@ -1486,54 +1465,54 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="31">
+      <c r="E19" s="28">
         <v>2021</v>
       </c>
-      <c r="F19" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="31">
+      <c r="F19" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="28">
         <v>2</v>
       </c>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="27" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="33" t="s">
+      <c r="C20" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="34">
+      <c r="E20" s="31">
         <v>2018</v>
       </c>
-      <c r="F20" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="34">
-        <v>4</v>
-      </c>
-      <c r="H20" s="33" t="s">
+      <c r="F20" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="31">
+        <v>4</v>
+      </c>
+      <c r="H20" s="30" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1597,7 +1576,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>49</v>
@@ -1632,7 +1611,7 @@
         <v>2018</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="G24" s="20">
         <v>4</v>
@@ -1649,7 +1628,7 @@
         <v>14</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>50</v>
@@ -1701,13 +1680,13 @@
         <v>20</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="E27" s="20">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="F27" s="13" t="s">
         <v>10</v>
@@ -1720,80 +1699,80 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="37" t="s">
+      <c r="C28" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="34">
+        <v>2021</v>
+      </c>
+      <c r="F28" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="34">
+        <v>2</v>
+      </c>
+      <c r="H28" s="33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="37" t="s">
         <v>40</v>
-      </c>
-      <c r="D28" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" s="37">
-        <v>2021</v>
-      </c>
-      <c r="F28" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" s="37">
-        <v>2</v>
-      </c>
-      <c r="H28" s="36" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="40" t="s">
-        <v>41</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E29" s="40">
+      <c r="E29" s="37">
         <v>2018</v>
       </c>
-      <c r="F29" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="G29" s="40">
-        <v>4</v>
-      </c>
-      <c r="H29" s="39" t="s">
+      <c r="F29" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="37">
+        <v>4</v>
+      </c>
+      <c r="H29" s="36" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="53" t="s">
+      <c r="A30" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="54" t="s">
+      <c r="B30" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="55" t="s">
+      <c r="C30" s="52" t="s">
         <v>40</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E30" s="55">
+      <c r="E30" s="52">
         <v>2017</v>
       </c>
-      <c r="F30" s="54" t="s">
-        <v>10</v>
-      </c>
-      <c r="G30" s="55">
-        <v>4</v>
-      </c>
-      <c r="H30" s="54" t="s">
+      <c r="F30" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="52">
+        <v>4</v>
+      </c>
+      <c r="H30" s="51" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1813,7 +1792,7 @@
       <c r="E31" s="21">
         <v>2019</v>
       </c>
-      <c r="F31" s="54" t="s">
+      <c r="F31" s="51" t="s">
         <v>10</v>
       </c>
       <c r="G31" s="21">
@@ -1857,7 +1836,7 @@
         <v>14</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>37</v>
@@ -1883,7 +1862,7 @@
         <v>14</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>37</v>
@@ -1954,54 +1933,54 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A37" s="41" t="s">
+      <c r="A37" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="42" t="s">
+      <c r="B37" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="D37" s="14" t="s">
+      <c r="C37" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="43">
+      <c r="E37" s="39">
         <v>2015</v>
       </c>
-      <c r="F37" s="43" t="s">
+      <c r="F37" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="G37" s="43">
+      <c r="G37" s="39">
         <v>2</v>
       </c>
-      <c r="H37" s="42" t="s">
+      <c r="H37" s="39" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A38" s="44" t="s">
+    <row r="38" spans="1:8">
+      <c r="A38" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="45" t="s">
+      <c r="B38" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="D38" s="45" t="s">
+      <c r="C38" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="E38" s="46">
+      <c r="E38" s="42">
         <v>2018</v>
       </c>
-      <c r="F38" s="15" t="s">
+      <c r="F38" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="G38" s="46">
-        <v>4</v>
-      </c>
-      <c r="H38" s="45" t="s">
+      <c r="G38" s="42">
+        <v>4</v>
+      </c>
+      <c r="H38" s="42" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2013,9 +1992,9 @@
         <v>14</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D39" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="15" t="s">
         <v>52</v>
       </c>
       <c r="E39" s="22">
@@ -2039,7 +2018,7 @@
         <v>14</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D40" s="15" t="s">
         <v>39</v>
@@ -2136,28 +2115,28 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A44" s="47" t="s">
+      <c r="A44" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="48" t="s">
+      <c r="B44" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C44" s="49" t="s">
+      <c r="C44" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D44" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="49">
+      <c r="E44" s="46">
         <v>2022</v>
       </c>
-      <c r="F44" s="48" t="s">
+      <c r="F44" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="G44" s="49">
-        <v>4</v>
-      </c>
-      <c r="H44" s="48" t="s">
+      <c r="G44" s="46">
+        <v>4</v>
+      </c>
+      <c r="H44" s="45" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed "Exceptions" Header/Column from Vehicle_Matrix
Updated UML image and file based on teacher comments
</commit_message>
<xml_diff>
--- a/doc/Vehicle_Matrix.xlsx
+++ b/doc/Vehicle_Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\PC\Misc\Documents\CIS255_Vehicle\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256B3944-1755-4C06-BD82-0045347248B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA371DE2-DCB4-43DF-B68C-41DF2572084E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="13740" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="52">
   <si>
     <t>Make</t>
   </si>
@@ -155,12 +155,6 @@
     <t>Model S</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Ranger</t>
   </si>
   <si>
@@ -168,9 +162,6 @@
   </si>
   <si>
     <t>Taurus</t>
-  </si>
-  <si>
-    <t>Exception</t>
   </si>
   <si>
     <t>Avenger</t>
@@ -495,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -606,16 +597,10 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -977,1166 +962,1033 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="16" customWidth="1"/>
-    <col min="16384" max="16384" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="16" customWidth="1"/>
+    <col min="16383" max="16383" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="48" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="48" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="49" t="s">
+      <c r="E1" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="G1" s="46" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:7" s="1" customFormat="1">
+      <c r="A2" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="54" t="s">
+      <c r="C2" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="55">
+      <c r="D2" s="53">
         <v>2018</v>
       </c>
-      <c r="F2" s="54" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="55">
+      <c r="E2" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="53">
         <v>2</v>
       </c>
-      <c r="H2" s="54" t="s">
+      <c r="G2" s="52" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="1" customFormat="1">
+    <row r="3" spans="1:7" s="1" customFormat="1">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="17">
+      <c r="D3" s="17">
         <v>2022</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="17">
+      <c r="F3" s="17">
         <v>2</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1">
+    <row r="4" spans="1:7" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="18">
+      <c r="C4" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="18">
         <v>2019</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="18">
-        <v>4</v>
-      </c>
-      <c r="H4" s="11" t="s">
+      <c r="E4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="18">
+        <v>4</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="1" customFormat="1">
+    <row r="5" spans="1:7" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="11" t="s">
+      <c r="C5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="18">
+      <c r="D5" s="18">
         <v>2016</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="18">
+      <c r="E5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="18">
         <v>2</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="G5" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="1" customFormat="1">
+    <row r="6" spans="1:7" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="18">
+      <c r="C6" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="18">
         <v>2016</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="18">
-        <v>4</v>
-      </c>
-      <c r="H6" s="11" t="s">
+      <c r="E6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="18">
+        <v>4</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1">
+    <row r="7" spans="1:7" s="1" customFormat="1">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="11" t="s">
+      <c r="C7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="18">
+      <c r="D7" s="18">
         <v>2015</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="18">
-        <v>4</v>
-      </c>
-      <c r="H7" s="11" t="s">
+      <c r="E7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="18">
+        <v>4</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1">
+    <row r="8" spans="1:7" s="1" customFormat="1">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="11" t="s">
+      <c r="C8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="18">
+      <c r="D8" s="18">
         <v>2018</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="18">
+      <c r="E8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="18">
         <v>2</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="G8" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1">
+    <row r="9" spans="1:7" s="1" customFormat="1">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="11" t="s">
+      <c r="C9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="18">
+      <c r="D9" s="18">
         <v>2019</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="18">
+      <c r="E9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="18">
         <v>2</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="G9" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A10" s="56" t="s">
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A10" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="58" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="57" t="s">
+      <c r="C10" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="58">
+      <c r="D10" s="56">
         <v>2020</v>
       </c>
-      <c r="F10" s="57" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="58">
+      <c r="E10" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="56">
         <v>2</v>
       </c>
-      <c r="H10" s="57" t="s">
+      <c r="G10" s="55" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:7">
       <c r="A11" s="23" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="24" t="s">
+      <c r="C11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="25">
+      <c r="D11" s="25">
         <v>2018</v>
       </c>
-      <c r="F11" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="25">
-        <v>4</v>
-      </c>
-      <c r="H11" s="24" t="s">
+      <c r="E11" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="25">
+        <v>4</v>
+      </c>
+      <c r="G11" s="24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:7">
       <c r="A12" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="12" t="s">
+      <c r="C12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="19">
+      <c r="D12" s="19">
         <v>2018</v>
       </c>
-      <c r="F12" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="19">
-        <v>4</v>
-      </c>
-      <c r="H12" s="12" t="s">
+      <c r="E12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="19">
+        <v>4</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:7">
       <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="12" t="s">
+      <c r="C13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="19">
+      <c r="D13" s="19">
         <v>2017</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="E13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="19">
-        <v>4</v>
-      </c>
-      <c r="H13" s="12" t="s">
+      <c r="F13" s="19">
+        <v>4</v>
+      </c>
+      <c r="G13" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:7">
       <c r="A14" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="12" t="s">
+      <c r="C14" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="19">
+      <c r="D14" s="19">
         <v>2016</v>
       </c>
-      <c r="F14" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="19">
-        <v>4</v>
-      </c>
-      <c r="H14" s="12" t="s">
+      <c r="E14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="19">
+        <v>4</v>
+      </c>
+      <c r="G14" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:7">
       <c r="A15" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="19">
+      <c r="C15" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="19">
         <v>2018</v>
       </c>
-      <c r="F15" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="19">
-        <v>4</v>
-      </c>
-      <c r="H15" s="12" t="s">
+      <c r="E15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="19">
+        <v>4</v>
+      </c>
+      <c r="G15" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:7">
       <c r="A16" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="19">
+      <c r="C16" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="19">
         <v>2014</v>
       </c>
-      <c r="F16" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="19">
-        <v>4</v>
-      </c>
-      <c r="H16" s="12" t="s">
+      <c r="E16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="19">
+        <v>4</v>
+      </c>
+      <c r="G16" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:7">
       <c r="A17" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="12" t="s">
+      <c r="C17" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="19">
+      <c r="D17" s="19">
         <v>2019</v>
       </c>
-      <c r="F17" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="19">
+      <c r="E17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="19">
         <v>2</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="G17" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:7">
       <c r="A18" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="12" t="s">
+      <c r="C18" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="19">
+      <c r="D18" s="19">
         <v>2020</v>
       </c>
-      <c r="F18" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="19">
+      <c r="E18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="19">
         <v>2</v>
       </c>
-      <c r="H18" s="12" t="s">
+      <c r="G18" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1">
+    <row r="19" spans="1:7" ht="15.75" thickBot="1">
       <c r="A19" s="26" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="27" t="s">
+      <c r="C19" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="28">
+      <c r="D19" s="28">
         <v>2021</v>
       </c>
-      <c r="F19" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="28">
+      <c r="E19" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="28">
         <v>2</v>
       </c>
-      <c r="H19" s="27" t="s">
+      <c r="G19" s="27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:7">
       <c r="A20" s="29" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="30" t="s">
+      <c r="C20" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="31">
+      <c r="D20" s="31">
         <v>2018</v>
       </c>
-      <c r="F20" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="31">
-        <v>4</v>
-      </c>
-      <c r="H20" s="30" t="s">
+      <c r="E20" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="31">
+        <v>4</v>
+      </c>
+      <c r="G20" s="30" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:7">
       <c r="A21" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="20">
+      <c r="C21" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="20">
         <v>2019</v>
       </c>
-      <c r="F21" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" s="20">
-        <v>4</v>
-      </c>
-      <c r="H21" s="13" t="s">
+      <c r="E21" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="20">
+        <v>4</v>
+      </c>
+      <c r="G21" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:7">
       <c r="A22" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="20">
+      <c r="C22" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="20">
         <v>2019</v>
       </c>
-      <c r="F22" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="20">
-        <v>4</v>
-      </c>
-      <c r="H22" s="13" t="s">
+      <c r="E22" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="20">
+        <v>4</v>
+      </c>
+      <c r="G22" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:7">
       <c r="A23" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="20">
+      <c r="C23" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="20">
         <v>2016</v>
       </c>
-      <c r="F23" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="20">
-        <v>4</v>
-      </c>
-      <c r="H23" s="13" t="s">
+      <c r="E23" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="20">
+        <v>4</v>
+      </c>
+      <c r="G23" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:7">
       <c r="A24" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B24" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="13" t="s">
+      <c r="C24" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="20">
+      <c r="D24" s="20">
         <v>2018</v>
       </c>
-      <c r="F24" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="20">
-        <v>4</v>
-      </c>
-      <c r="H24" s="13" t="s">
+      <c r="E24" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="20">
+        <v>4</v>
+      </c>
+      <c r="G24" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:7">
       <c r="A25" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="20">
+      <c r="C25" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="20">
         <v>2019</v>
       </c>
-      <c r="F25" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" s="20">
-        <v>4</v>
-      </c>
-      <c r="H25" s="13" t="s">
+      <c r="E25" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="20">
+        <v>4</v>
+      </c>
+      <c r="G25" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:7">
       <c r="A26" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="13">
+      <c r="C26" s="13">
         <v>86</v>
       </c>
-      <c r="E26" s="20">
+      <c r="D26" s="20">
         <v>2019</v>
       </c>
-      <c r="F26" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" s="20">
+      <c r="E26" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="20">
         <v>2</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="G26" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:7">
       <c r="A27" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E27" s="20">
+      <c r="C27" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="20">
         <v>2023</v>
       </c>
-      <c r="F27" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="20">
+      <c r="E27" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="20">
         <v>2</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="G27" s="13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1">
+    <row r="28" spans="1:7" ht="15.75" thickBot="1">
       <c r="A28" s="32" t="s">
         <v>30</v>
       </c>
       <c r="B28" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="33" t="s">
+      <c r="C28" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="34">
+      <c r="D28" s="34">
         <v>2021</v>
       </c>
-      <c r="F28" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" s="34">
+      <c r="E28" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="34">
         <v>2</v>
       </c>
-      <c r="H28" s="33" t="s">
+      <c r="G28" s="33" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:7">
       <c r="A29" s="35" t="s">
         <v>34</v>
       </c>
       <c r="B29" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="14" t="s">
+      <c r="C29" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E29" s="37">
+      <c r="D29" s="37">
         <v>2018</v>
       </c>
-      <c r="F29" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="G29" s="37">
-        <v>4</v>
-      </c>
-      <c r="H29" s="36" t="s">
+      <c r="E29" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="37">
+        <v>4</v>
+      </c>
+      <c r="G29" s="36" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="50" t="s">
+    <row r="30" spans="1:7">
+      <c r="A30" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="51" t="s">
+      <c r="B30" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="14" t="s">
+      <c r="C30" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E30" s="52">
+      <c r="D30" s="50">
         <v>2017</v>
       </c>
-      <c r="F30" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="G30" s="52">
-        <v>4</v>
-      </c>
-      <c r="H30" s="51" t="s">
+      <c r="E30" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="50">
+        <v>4</v>
+      </c>
+      <c r="G30" s="49" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:7">
       <c r="A31" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" s="14" t="s">
+      <c r="C31" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E31" s="21">
+      <c r="D31" s="21">
         <v>2019</v>
       </c>
-      <c r="F31" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="G31" s="21">
-        <v>4</v>
-      </c>
-      <c r="H31" s="14" t="s">
+      <c r="E31" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="21">
+        <v>4</v>
+      </c>
+      <c r="G31" s="14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:7">
       <c r="A32" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B32" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D32" s="14" t="s">
+      <c r="C32" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E32" s="21">
+      <c r="D32" s="21">
         <v>2016</v>
       </c>
-      <c r="F32" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G32" s="21">
-        <v>4</v>
-      </c>
-      <c r="H32" s="14" t="s">
+      <c r="E32" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="21">
+        <v>4</v>
+      </c>
+      <c r="G32" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:7">
       <c r="A33" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D33" s="14" t="s">
+      <c r="C33" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E33" s="21">
+      <c r="D33" s="21">
         <v>2015</v>
       </c>
-      <c r="F33" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G33" s="21">
-        <v>4</v>
-      </c>
-      <c r="H33" s="14" t="s">
+      <c r="E33" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="21">
+        <v>4</v>
+      </c>
+      <c r="G33" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:7">
       <c r="A34" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B34" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D34" s="14" t="s">
+      <c r="C34" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E34" s="21">
+      <c r="D34" s="21">
         <v>2015</v>
       </c>
-      <c r="F34" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G34" s="21">
-        <v>4</v>
-      </c>
-      <c r="H34" s="14" t="s">
+      <c r="E34" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="21">
+        <v>4</v>
+      </c>
+      <c r="G34" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:7">
       <c r="A35" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35" s="14" t="s">
+      <c r="C35" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E35" s="21">
+      <c r="D35" s="21">
         <v>2012</v>
       </c>
-      <c r="F35" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G35" s="21">
+      <c r="E35" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="21">
         <v>2</v>
       </c>
-      <c r="H35" s="14" t="s">
+      <c r="G35" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:7">
       <c r="A36" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B36" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E36" s="21">
+      <c r="C36" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="21">
         <v>2013</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="E36" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G36" s="21">
+      <c r="F36" s="21">
         <v>2</v>
       </c>
-      <c r="H36" s="14" t="s">
+      <c r="G36" s="14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15.75" thickBot="1">
+    <row r="37" spans="1:7" ht="15.75" thickBot="1">
       <c r="A37" s="38" t="s">
         <v>34</v>
       </c>
       <c r="B37" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="D37" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="E37" s="39">
+      <c r="C37" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="39">
         <v>2015</v>
       </c>
-      <c r="F37" s="39" t="s">
+      <c r="E37" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="G37" s="39">
+      <c r="F37" s="39">
         <v>2</v>
       </c>
-      <c r="H37" s="39" t="s">
+      <c r="G37" s="39" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="41" t="s">
+    <row r="38" spans="1:7">
+      <c r="A38" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="42" t="s">
+      <c r="B38" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="E38" s="42">
+      <c r="C38" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="41">
         <v>2018</v>
       </c>
-      <c r="F38" s="42" t="s">
+      <c r="E38" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="G38" s="42">
-        <v>4</v>
-      </c>
-      <c r="H38" s="42" t="s">
+      <c r="F38" s="41">
+        <v>4</v>
+      </c>
+      <c r="G38" s="41" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:7">
       <c r="A39" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E39" s="22">
+      <c r="C39" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" s="22">
         <v>2023</v>
       </c>
-      <c r="F39" s="15" t="s">
+      <c r="E39" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G39" s="22">
-        <v>4</v>
-      </c>
-      <c r="H39" s="15" t="s">
+      <c r="F39" s="22">
+        <v>4</v>
+      </c>
+      <c r="G39" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:7">
       <c r="A40" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D40" s="15" t="s">
+      <c r="C40" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E40" s="22">
+      <c r="D40" s="22">
         <v>2021</v>
       </c>
-      <c r="F40" s="15" t="s">
+      <c r="E40" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G40" s="22">
-        <v>4</v>
-      </c>
-      <c r="H40" s="15" t="s">
+      <c r="F40" s="22">
+        <v>4</v>
+      </c>
+      <c r="G40" s="15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:7">
       <c r="A41" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D41" s="15" t="s">
+      <c r="C41" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E41" s="22">
+      <c r="D41" s="22">
         <v>2021</v>
       </c>
-      <c r="F41" s="15" t="s">
+      <c r="E41" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G41" s="22">
-        <v>4</v>
-      </c>
-      <c r="H41" s="15" t="s">
+      <c r="F41" s="22">
+        <v>4</v>
+      </c>
+      <c r="G41" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:7">
       <c r="A42" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D42" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E42" s="22">
+      <c r="C42" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="22">
         <v>2021</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="E42" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G42" s="22">
-        <v>4</v>
-      </c>
-      <c r="H42" s="15" t="s">
+      <c r="F42" s="22">
+        <v>4</v>
+      </c>
+      <c r="G42" s="15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:7">
       <c r="A43" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B43" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E43" s="22">
+      <c r="C43" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" s="22">
         <v>2020</v>
       </c>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G43" s="22">
-        <v>4</v>
-      </c>
-      <c r="H43" s="15" t="s">
+      <c r="F43" s="22">
+        <v>4</v>
+      </c>
+      <c r="G43" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A44" s="44" t="s">
+    <row r="44" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A44" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="45" t="s">
+      <c r="B44" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C44" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="D44" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="E44" s="46">
+      <c r="C44" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" s="44">
         <v>2022</v>
       </c>
-      <c r="F44" s="45" t="s">
+      <c r="E44" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="G44" s="46">
-        <v>4</v>
-      </c>
-      <c r="H44" s="45" t="s">
+      <c r="F44" s="44">
+        <v>4</v>
+      </c>
+      <c r="G44" s="43" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated file structure with folder addition "bin" for temporary storage of unused files
Updated ReadMe files to reflect change from visio to draw.io
</commit_message>
<xml_diff>
--- a/doc/Vehicle_Matrix.xlsx
+++ b/doc/Vehicle_Matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\PC\Misc\Documents\CIS255_Vehicle\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA371DE2-DCB4-43DF-B68C-41DF2572084E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC197E9-DE9F-42EC-98DC-2A30C5E89190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="13740" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -965,7 +965,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>

</xml_diff>

<commit_message>
Revised Diversity: Coupe #2 issues regarding Honda Coupe Options
</commit_message>
<xml_diff>
--- a/doc/Vehicle_Matrix.xlsx
+++ b/doc/Vehicle_Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\PC\Misc\Documents\CIS255_Vehicle\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC197E9-DE9F-42EC-98DC-2A30C5E89190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB5CE3F-27EB-47C1-A864-488420DA9241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="13740" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -965,7 +965,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
@@ -1793,13 +1793,13 @@
         <v>20</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D36" s="21">
         <v>2013</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F36" s="21">
         <v>2</v>

</xml_diff>

<commit_message>
Revert "Revised Diversity: Coupe #2 issues regarding Honda Coupe Options"
This reverts commit 1b1ab200cccd4f0af7aaf35b9db244e2f002475b.
</commit_message>
<xml_diff>
--- a/doc/Vehicle_Matrix.xlsx
+++ b/doc/Vehicle_Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\PC\Misc\Documents\CIS255_Vehicle\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB5CE3F-27EB-47C1-A864-488420DA9241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC197E9-DE9F-42EC-98DC-2A30C5E89190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="13740" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -965,7 +965,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
@@ -1793,13 +1793,13 @@
         <v>20</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D36" s="21">
         <v>2013</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F36" s="21">
         <v>2</v>

</xml_diff>